<commit_message>
My first ReFrameWork project for Naukri recruitment proess..
</commit_message>
<xml_diff>
--- a/Naukri/Results/NaukriSearch.xlsx
+++ b/Naukri/Results/NaukriSearch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sundarsi\source\RPA\UiPath\github\Naukri\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D210FC95-926C-400E-AC1D-F779E587B6F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69CA64F-4FD5-469E-A1B6-6EE8BC6ADFFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{82030CAF-2DF0-485D-945C-EB60E8957052}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" xr2:uid="{82030CAF-2DF0-485D-945C-EB60E8957052}"/>
   </bookViews>
   <sheets>
     <sheet name="NaukriSearch" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Slno</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>4-7</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Asp.net, C#</t>
+  </si>
+  <si>
+    <t>4-6</t>
   </si>
 </sst>
 </file>
@@ -474,14 +483,14 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
@@ -528,23 +537,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="I2">
         <v>10</v>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80649DEF-4029-4535-A402-38E1263CE580}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,6 +636,33 @@
         <v>14</v>
       </c>
     </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4">
+        <v>50</v>
+      </c>
+      <c r="I3" s="3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>